<commit_message>
Busqueda y flujos del Gestionar cupo + Circuto
</commit_message>
<xml_diff>
--- a/External Resources/UI/Integracion/CasosPruebaCircuitos.xlsx
+++ b/External Resources/UI/Integracion/CasosPruebaCircuitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio.olivieri\RobotTesting\YARD\External Resources\UI\Integracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDD5F56-CAB4-4072-8CAD-4EE43DDF68CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29D255F-7D17-46A4-BFBE-E9BEC6D7BC55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="507" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="2505" windowWidth="15375" windowHeight="7875" tabRatio="507" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Circuitos" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>${CodProducto}</t>
   </si>
@@ -81,9 +81,6 @@
     <t>${ConWSAfip}</t>
   </si>
   <si>
-    <t>Se aceptó el ingreso de la descarga</t>
-  </si>
-  <si>
     <t>${ConTarjeta}</t>
   </si>
   <si>
@@ -99,7 +96,13 @@
     <t>${NroCircuito}</t>
   </si>
   <si>
-    <t>Circuito: Validar Cupo OK / …</t>
+    <t>Circuito: Validar Cupo Pendiente / anular movimiento</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>La descarga quedó en estado Pendiente</t>
   </si>
 </sst>
 </file>
@@ -504,7 +507,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,10 +518,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -526,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -538,9 +541,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +573,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -621,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
@@ -630,10 +633,10 @@
         <v>15</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>17</v>
@@ -644,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>888811111152</v>
+        <v>888811111154</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -696,10 +699,14 @@
       <c r="T2" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
+      <c r="U2" s="3">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="W2" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>